<commit_message>
Se agrego descripcion proyecto 0008-javacode-503
</commit_message>
<xml_diff>
--- a/Proyectos.xlsx
+++ b/Proyectos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="92">
   <si>
     <t>0002-javacode-503-plantilla</t>
   </si>
@@ -320,6 +320,30 @@
 Post Construct. Inicializa la clase y datos.
 Setter y getter de todas las variables.
 </t>
+  </si>
+  <si>
+    <t>0008-Javacode-503-SelectOneMenu-JSF-Hibernate</t>
+  </si>
+  <si>
+    <t>demobd</t>
+  </si>
+  <si>
+    <t>tbpais</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>Primefaces.5.</t>
+  </si>
+  <si>
+    <t>Hibernate,5.4.30. Clases dao,impl.</t>
+  </si>
+  <si>
+    <t>Beans: BeanPais.</t>
+  </si>
+  <si>
+    <t>FUNCIONA CON EL CONECTOR MYSQL 5,1,42.</t>
   </si>
 </sst>
 </file>
@@ -431,7 +455,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -460,6 +484,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -733,7 +760,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -741,13 +768,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="10.5"/>
@@ -942,136 +969,158 @@
       <c r="L5" s="11"/>
       <c r="M5" s="11"/>
     </row>
-    <row r="6" spans="1:13" s="7" customFormat="1" ht="221" customHeight="1">
+    <row r="6" spans="1:13" s="7" customFormat="1" ht="36.5" customHeight="1">
       <c r="A6" s="6" t="s">
-        <v>3</v>
+        <v>84</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>61</v>
+        <v>89</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>62</v>
+        <v>90</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F6" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="L6" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="M6" s="15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="7" customFormat="1" ht="221" customHeight="1">
+      <c r="A7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G7" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I7" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="J7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="6" t="s">
+      <c r="K7" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="L6" s="6" t="s">
+      <c r="L7" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="M6" s="6" t="s">
+      <c r="M7" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="3" t="s">
+    <row r="8" spans="1:13">
+      <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B8" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-    </row>
-    <row r="8" spans="1:13" s="14" customFormat="1" ht="42">
-      <c r="A8" s="13" t="s">
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+    </row>
+    <row r="9" spans="1:13" s="14" customFormat="1" ht="42">
+      <c r="A9" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B9" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C9" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="13" t="s">
+      <c r="D9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F9" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G9" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="H8" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="J8" s="13" t="s">
+      <c r="H9" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="K8" s="6" t="s">
+      <c r="K9" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="L8" s="13" t="s">
+      <c r="L9" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="M8" s="6" t="s">
+      <c r="M9" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="168">
-      <c r="A9" s="6" t="s">
+    <row r="10" spans="1:13" ht="168">
+      <c r="A10" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B10" s="12" t="s">
         <v>74</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-    </row>
-    <row r="10" spans="1:13" ht="115.5">
-      <c r="A10" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>75</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -1085,57 +1134,61 @@
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="1:13" ht="147.5" customHeight="1">
+    <row r="11" spans="1:13" ht="115.5">
       <c r="A11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+    </row>
+    <row r="12" spans="1:13" ht="147.5" customHeight="1">
+      <c r="A12" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B12" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C12" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D12" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F12" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G12" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="I12" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="J11" s="6" t="s">
+      <c r="J12" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="K11" s="6" t="s">
+      <c r="K12" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="3"/>
@@ -1316,6 +1369,21 @@
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
se agrego al excel el proyecto 0014-javacode-503
</commit_message>
<xml_diff>
--- a/Proyectos.xlsx
+++ b/Proyectos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="109">
   <si>
     <t>0002-javacode-503-plantilla</t>
   </si>
@@ -344,6 +344,57 @@
   </si>
   <si>
     <t>FUNCIONA CON EL CONECTOR MYSQL 5,1,42.</t>
+  </si>
+  <si>
+    <t>0010-Javacode-503-Crud-Mvc-Jsf-Hibernate-Primefaces</t>
+  </si>
+  <si>
+    <t>0012-javacode-503-Reportes-Java-Web</t>
+  </si>
+  <si>
+    <t>bdempleado</t>
+  </si>
+  <si>
+    <t>tbempleado, tbdepartamento, tbmunicipio, tbpais</t>
+  </si>
+  <si>
+    <t>empleadoBean</t>
+  </si>
+  <si>
+    <t>SON DOS PROYECTOS: ejemploReporte, exportarReporte. Se agrego plugins de Ireport, en el cual se creo la conexión a la base mysql bdreporte</t>
+  </si>
+  <si>
+    <t>clienteBean</t>
+  </si>
+  <si>
+    <t>bdreporte</t>
+  </si>
+  <si>
+    <t>cliente</t>
+  </si>
+  <si>
+    <t>librerias de Ireport, y se instalo plugins de Ireports en netbeans.</t>
+  </si>
+  <si>
+    <t>0014-Javacode-503-Sistema-Facturacion-Web</t>
+  </si>
+  <si>
+    <t>facturacion</t>
+  </si>
+  <si>
+    <t>Hibernate: 5.4:30, mysql.connector-java-5.1.42.bin.jar. PLUGIN IREPORT</t>
+  </si>
+  <si>
+    <t>cliente, detallefactura, factura, producto, usuario, vendedor</t>
+  </si>
+  <si>
+    <t>tiene pantallas de logueo, con usuario/password en tablas</t>
+  </si>
+  <si>
+    <t>index, login, plantilla, factura, producto,vendedor, factura</t>
+  </si>
+  <si>
+    <t>clienteBean,facturaBean,loginBean,productoBean,vendedorBean</t>
   </si>
 </sst>
 </file>
@@ -455,7 +506,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -487,6 +538,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -768,13 +828,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="10.5"/>
@@ -1010,139 +1070,181 @@
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="7" customFormat="1" ht="221" customHeight="1">
+    <row r="7" spans="1:13" s="7" customFormat="1" ht="44" customHeight="1">
       <c r="A7" s="6" t="s">
-        <v>3</v>
+        <v>92</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>61</v>
+        <v>89</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>62</v>
+        <v>96</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F7" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="L7" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="M7" s="15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="7" customFormat="1" ht="36.5" customHeight="1">
+      <c r="A8" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" s="7" customFormat="1" ht="75.5" customHeight="1">
+      <c r="A9" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="M9" s="15" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" s="7" customFormat="1" ht="221" customHeight="1">
+      <c r="A10" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G10" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I10" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="J10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="K7" s="6" t="s">
+      <c r="K10" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="L7" s="6" t="s">
+      <c r="L10" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="M7" s="6" t="s">
+      <c r="M10" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
-      <c r="A8" s="3" t="s">
+    <row r="11" spans="1:13">
+      <c r="A11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-    </row>
-    <row r="9" spans="1:13" s="14" customFormat="1" ht="42">
-      <c r="A9" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="H9" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I9" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="J9" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="L9" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="M9" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="168">
-      <c r="A10" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-    </row>
-    <row r="11" spans="1:13" ht="115.5">
-      <c r="A11" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -1153,46 +1255,54 @@
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
     </row>
-    <row r="12" spans="1:13" ht="147.5" customHeight="1">
-      <c r="A12" s="6" t="s">
-        <v>8</v>
+    <row r="12" spans="1:13" s="14" customFormat="1" ht="42">
+      <c r="A12" s="13" t="s">
+        <v>5</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="E12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="6" t="s">
-        <v>78</v>
+      <c r="F12" s="13" t="s">
+        <v>68</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="J12" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12" s="13" t="s">
         <v>70</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
+        <v>73</v>
+      </c>
+      <c r="L12" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="168">
+      <c r="A13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>74</v>
+      </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -1205,9 +1315,13 @@
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
     </row>
-    <row r="14" spans="1:13">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
+    <row r="14" spans="1:13" ht="115.5">
+      <c r="A14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>75</v>
+      </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -1220,20 +1334,42 @@
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
     </row>
-    <row r="15" spans="1:13">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
+    <row r="15" spans="1:13" ht="147.5" customHeight="1">
+      <c r="A15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
     </row>
     <row r="16" spans="1:13">
       <c r="A16" s="3"/>
@@ -1385,6 +1521,51 @@
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
     </row>
+    <row r="26" spans="1:13">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -1393,17 +1574,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="41.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.36328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.453125" style="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.7265625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.1796875" bestFit="1" customWidth="1"/>
   </cols>
@@ -1421,7 +1602,7 @@
       <c r="D1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="16" t="s">
         <v>27</v>
       </c>
       <c r="F1" s="8" t="s">
@@ -1447,7 +1628,7 @@
       <c r="D2" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="17" t="s">
         <v>26</v>
       </c>
       <c r="F2" s="9" t="s">
@@ -1514,7 +1695,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>84</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>29</v>
@@ -1526,7 +1707,7 @@
         <v>33</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>36</v>
@@ -1540,7 +1721,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>92</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>29</v>
@@ -1552,7 +1733,7 @@
         <v>33</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>53</v>
+        <v>94</v>
       </c>
       <c r="F6" s="10" t="s">
         <v>36</v>
@@ -1566,7 +1747,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>93</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>29</v>
@@ -1578,7 +1759,7 @@
         <v>33</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>68</v>
+        <v>99</v>
       </c>
       <c r="F7" s="10" t="s">
         <v>36</v>
@@ -1592,19 +1773,19 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>102</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>36</v>
+        <v>103</v>
       </c>
       <c r="F8" s="10" t="s">
         <v>36</v>
@@ -1618,19 +1799,19 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="F9" s="10" t="s">
         <v>36</v>
@@ -1644,7 +1825,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>29</v>
@@ -1656,7 +1837,7 @@
         <v>33</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="F10" s="10" t="s">
         <v>36</v>
@@ -1669,14 +1850,118 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
+      <c r="A11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>